<commit_message>
DataFiles for Revenue Prediction Model, Singapore and Indonesia
</commit_message>
<xml_diff>
--- a/SystemCode/Data Exploration/ParkwayPayment_DataDictionary.xlsx
+++ b/SystemCode/Data Exploration/ParkwayPayment_DataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://parkwaypantailimited-my.sharepoint.com/personal/harry_chan_parkwaypantai_com/Documents/Education/ISS_Master/Project/Semester2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PRS-PM-ISY5002-GROUP5\SystemCode\Data Exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{01185D22-9988-437D-92BA-60A1CE2EC756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E28E9BE-70E5-4096-A922-114891AF5ED9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2118F4B9-3B6C-4FF3-A77F-B7677EECA9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaymentData" sheetId="11" r:id="rId1"/>
@@ -2538,18 +2538,18 @@
   </sheetPr>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="79.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="183" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="183" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>67</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>73</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>74</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>75</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>76</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>77</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>78</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>82</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>83</v>
       </c>
@@ -3489,17 +3489,17 @@
   </sheetPr>
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>83</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>83</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>86</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>88</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>90</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>92</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>98</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>100</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>102</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>104</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>106</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>108</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>108</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>111</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>113</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>115</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>117</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>119</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>121</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>123</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>125</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>127</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>129</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>131</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>133</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>135</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>137</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>139</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>141</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>143</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>145</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>147</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>149</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>151</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>153</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>155</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>157</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>159</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>161</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>163</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>165</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>167</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>169</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>171</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>171</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>174</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>176</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>178</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>180</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>184</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>186</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>188</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>190</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>190</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>193</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>195</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>197</v>
       </c>
@@ -3995,7 +3995,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>197</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>200</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>202</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>204</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>206</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>208</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>210</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>210</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>213</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>215</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>217</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>219</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>221</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>223</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>223</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>226</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>228</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>230</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>232</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>234</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>236</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>238</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>240</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>242</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>244</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>246</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>248</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>248</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>250</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>252</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>254</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>256</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>258</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>260</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>262</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>264</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>266</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>267</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>269</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>271</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>273</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>275</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>276</v>
       </c>
@@ -4350,19 +4350,19 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F7:F8"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>278</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>280</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>282</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>284</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>286</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>288</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>290</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>292</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>294</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>296</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>298</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>300</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>302</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>304</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>306</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>308</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>310</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>312</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>314</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>316</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>318</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>320</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>322</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>324</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>326</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>328</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>330</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>332</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>334</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>336</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>338</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>340</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>342</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>344</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>346</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>348</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>350</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>352</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>354</v>
       </c>
@@ -4682,401 +4682,401 @@
         <v>355</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>360</v>
+        <v>131</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>388</v>
-      </c>
       <c r="B60" s="6" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>131</v>
+        <v>391</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>391</v>
+        <v>328</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>328</v>
+        <v>394</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+      <c r="B65" s="6"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="B66" s="6"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>432</v>
+        <v>346</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>346</v>
+        <v>435</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="B91" s="6" t="s">
         <v>444</v>
       </c>
     </row>
@@ -5087,6 +5087,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BEA8BB570139144988694C3AEC80FE2F" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbda8aa845f0a3db0246a87301d6b0d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="24f65403-8f48-41bc-98c5-be11f8236bb7" xmlns:ns3="875f46df-add5-4fd9-babe-87bea569ca8d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="642b582dab4a2cc370770f29bfb39edf" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5294,25 +5312,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF255EDD-F4A5-41C0-BF18-33858FE3FB55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="79125d09-4ad7-46e8-a862-3fdf877307d5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc0b5052-816d-429d-9486-53efd02ce9e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EE94AE-FAB3-4F21-9B2B-7794A64A2427}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{304E51DA-D5F6-4914-ABF1-B25C0C0BFF05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5330,30 +5356,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8EE94AE-FAB3-4F21-9B2B-7794A64A2427}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF255EDD-F4A5-41C0-BF18-33858FE3FB55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="79125d09-4ad7-46e8-a862-3fdf877307d5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc0b5052-816d-429d-9486-53efd02ce9e2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>